<commit_message>
Small Changes to instructions
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -941,7 +941,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -967,8 +967,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1833,318 +1839,319 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="5.25" style="11" customWidth="1"/>
     <col min="3" max="3" width="11" style="12" customWidth="1"/>
-    <col min="4" max="4" width="41.375" customWidth="1"/>
-    <col min="5" max="5" width="9" style="14"/>
+    <col min="4" max="4" width="58.5" customWidth="1"/>
+    <col min="5" max="5" width="9" style="13"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="4" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="E2" s="19"/>
+    </row>
+    <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="19" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="19" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="15" t="s">
         <v>152</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="19" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="14" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="19" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="19" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="19" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="19" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="19" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="19" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="19" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
+    <row r="16" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
+    <row r="18" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="4" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2335,20 +2342,20 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
+    <row r="31" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="16">
         <v>30</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="16" t="s">
         <v>253</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Extract display to separate class
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -941,7 +941,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -970,9 +970,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -1839,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1864,7 +1861,7 @@
       <c r="D2" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E2" s="19"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -1879,7 +1876,7 @@
       <c r="D3" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="16" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1896,7 +1893,7 @@
       <c r="D4" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="16" t="s">
         <v>146</v>
       </c>
     </row>
@@ -1913,7 +1910,7 @@
       <c r="D5" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="16" t="s">
         <v>150</v>
       </c>
     </row>
@@ -1930,7 +1927,7 @@
       <c r="D6" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="16" t="s">
         <v>154</v>
       </c>
     </row>
@@ -1947,7 +1944,7 @@
       <c r="D7" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="16" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1964,7 +1961,7 @@
       <c r="D8" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="16" t="s">
         <v>158</v>
       </c>
     </row>
@@ -1981,7 +1978,7 @@
       <c r="D9" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="16" t="s">
         <v>164</v>
       </c>
     </row>
@@ -1998,7 +1995,7 @@
       <c r="D10" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E10" s="19" t="s">
+      <c r="E10" s="16" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2015,7 +2012,7 @@
       <c r="D11" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="16" t="s">
         <v>172</v>
       </c>
     </row>
@@ -2029,10 +2026,10 @@
       <c r="C12" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="E12" s="16" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2049,7 +2046,7 @@
       <c r="D13" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="16" t="s">
         <v>180</v>
       </c>
     </row>
@@ -2066,7 +2063,7 @@
       <c r="D14" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="16" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2155,275 +2152,275 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
+    <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="14" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
+    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="4" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
+    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
+    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="14" t="s">
         <v>219</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="4" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
+    <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
+    <row r="26" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="4" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
+    <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="4" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="14" t="s">
         <v>239</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="4" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
+    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="4" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="14" t="s">
         <v>247</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="4" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="16">
+    <row r="31" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="4" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
+    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="14" t="s">
         <v>254</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
+    <row r="33" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="11" t="s">
+      <c r="B33" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
+    <row r="34" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="4" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="35" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="4" t="s">
         <v>270</v>
       </c>
     </row>

</xml_diff>